<commit_message>
files are addded directley
branch1 branch for which teh new iteration of the released
</commit_message>
<xml_diff>
--- a/src/excel/assigneng.xlsx
+++ b/src/excel/assigneng.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="25">
   <si>
     <t>AssignId</t>
   </si>
@@ -76,6 +76,21 @@
   </si>
   <si>
     <t>Trading</t>
+  </si>
+  <si>
+    <t>Assigner</t>
+  </si>
+  <si>
+    <t>ds</t>
+  </si>
+  <si>
+    <t>assigneng4</t>
+  </si>
+  <si>
+    <t>wheels india</t>
+  </si>
+  <si>
+    <t>once a week</t>
   </si>
 </sst>
 </file>
@@ -416,10 +431,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -432,7 +447,7 @@
     <col min="6" max="6" width="18.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -451,8 +466,11 @@
       <c r="F1" t="s">
         <v>16</v>
       </c>
+      <c r="G1" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -471,8 +489,11 @@
       <c r="F2" t="s">
         <v>17</v>
       </c>
+      <c r="G2" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -491,8 +512,11 @@
       <c r="F3" t="s">
         <v>18</v>
       </c>
+      <c r="G3" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -510,6 +534,32 @@
       </c>
       <c r="F4" t="s">
         <v>19</v>
+      </c>
+      <c r="G4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="1">
+        <v>43132</v>
+      </c>
+      <c r="E5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>